<commit_message>
Second Day of DSA series
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rinku\Desktop\coding\FAANG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE52E2D5-AAA3-4AF8-BCD5-C08E14890B8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A09A15-218E-42EF-9D16-6B496F24E1FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1431,17 +1431,17 @@
     <t xml:space="preserve"> yes</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>Array  *</t>
+  </si>
+  <si>
+    <t>not opening</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1511,6 +1511,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1533,7 +1549,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1561,6 +1577,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1878,8 +1896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="16.100000000000001"/>
@@ -1917,7 +1935,7 @@
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="11" t="s">
@@ -1928,7 +1946,7 @@
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -1939,7 +1957,7 @@
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="11" t="s">
@@ -1950,7 +1968,7 @@
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="11" t="s">
@@ -1961,7 +1979,7 @@
       <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="11" t="s">
@@ -1972,7 +1990,7 @@
       <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -1983,7 +2001,7 @@
       <c r="A12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="11" t="s">
@@ -1994,7 +2012,7 @@
       <c r="A13" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -2005,7 +2023,7 @@
       <c r="A14" s="5" t="s">
         <v>466</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="13" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="11" t="s">
@@ -2016,7 +2034,7 @@
       <c r="A15" s="5" t="s">
         <v>466</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="11" t="s">
@@ -2027,7 +2045,7 @@
       <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="11" t="s">
@@ -2036,20 +2054,20 @@
     </row>
     <row r="17" spans="1:3" ht="21.05">
       <c r="A17" s="5" t="s">
-        <v>469</v>
-      </c>
-      <c r="B17" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="B17" s="13" t="s">
         <v>17</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="21.05">
       <c r="A18" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="11" t="s">
@@ -2060,7 +2078,7 @@
       <c r="A19" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="11" t="s">
@@ -2071,7 +2089,7 @@
       <c r="A20" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="11" t="s">
@@ -2082,7 +2100,7 @@
       <c r="A21" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -2093,7 +2111,7 @@
       <c r="A22" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="14" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="11" t="s">
@@ -2104,7 +2122,7 @@
       <c r="A23" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C23" s="11" t="s">
@@ -2115,7 +2133,7 @@
       <c r="A24" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="14" t="s">
         <v>24</v>
       </c>
       <c r="C24" s="11" t="s">
@@ -2126,7 +2144,7 @@
       <c r="A25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="11" t="s">
@@ -2137,7 +2155,7 @@
       <c r="A26" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="14" t="s">
         <v>26</v>
       </c>
       <c r="C26" s="11" t="s">
@@ -2148,7 +2166,7 @@
       <c r="A27" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C27" s="11" t="s">
@@ -2159,7 +2177,7 @@
       <c r="A28" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="14" t="s">
         <v>28</v>
       </c>
       <c r="C28" s="11" t="s">
@@ -2170,7 +2188,7 @@
       <c r="A29" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="14" t="s">
         <v>29</v>
       </c>
       <c r="C29" s="11" t="s">
@@ -2181,128 +2199,128 @@
       <c r="A30" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="14" t="s">
         <v>30</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="21.05">
       <c r="A31" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="21.05">
       <c r="A32" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="14" t="s">
         <v>32</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="21.05">
       <c r="A33" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="14" t="s">
         <v>33</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="21.05">
       <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="21.05">
       <c r="A35" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="21.05">
       <c r="A36" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="14" t="s">
         <v>36</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="21.05">
       <c r="A37" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="13" t="s">
         <v>37</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>4</v>
+        <v>469</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="21.05">
       <c r="A38" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="14" t="s">
         <v>38</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="21.05">
       <c r="A39" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="14" t="s">
         <v>39</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="21.05">
       <c r="A40" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="14" t="s">
         <v>40</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="21.05">
       <c r="A41" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B41" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="B41" s="13" t="s">
         <v>41</v>
       </c>
       <c r="C41" s="11" t="s">

</xml_diff>

<commit_message>
Third Day of DSA series
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rinku\Desktop\coding\FAANG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496FBD86-AFEE-4E0D-A48F-D289778C1F6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE422A9E-39D2-46B2-98B9-07905D92A6B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="472">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1437,14 +1437,17 @@
     <t>not opening</t>
   </si>
   <si>
-    <t>no</t>
+    <t>Matrix *</t>
+  </si>
+  <si>
+    <t>not clear</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1530,6 +1533,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1552,7 +1562,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1587,6 +1597,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1904,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="16.100000000000001"/>
@@ -2332,7 +2344,7 @@
         <v>41</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="21.05">
@@ -2402,24 +2414,24 @@
     </row>
     <row r="49" spans="1:3" ht="21.05">
       <c r="A49" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B49" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="B49" s="16" t="s">
         <v>48</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="21.05">
       <c r="A50" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="13" t="s">
         <v>49</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="21.05">
@@ -2468,77 +2480,77 @@
       <c r="A56" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="13" t="s">
         <v>54</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="21.05">
       <c r="A57" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="13" t="s">
         <v>55</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="21.05">
       <c r="A58" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B58" s="13" t="s">
         <v>56</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="21.05">
       <c r="A59" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="17" t="s">
         <v>57</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="21.05">
       <c r="A60" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B60" s="13" t="s">
         <v>58</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="21.05">
       <c r="A61" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B61" s="16" t="s">
         <v>59</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>4</v>
+        <v>471</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="21.05">
       <c r="A62" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="B62" s="13" t="s">
         <v>60</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="21.05">
@@ -5197,11 +5209,11 @@
       <c r="A312" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="B312" s="6" t="s">
+      <c r="B312" s="13" t="s">
         <v>302</v>
       </c>
       <c r="C312" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="313" spans="1:3" ht="21.05">

</xml_diff>

<commit_message>
Fourth Day Of DSA series
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rinku\Desktop\coding\FAANG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE422A9E-39D2-46B2-98B9-07905D92A6B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C2F115-686D-44C9-8DEE-DA4947B0C4A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="473">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1441,6 +1441,9 @@
   </si>
   <si>
     <t>not clear</t>
+  </si>
+  <si>
+    <t>String *</t>
   </si>
 </sst>
 </file>
@@ -1916,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C501"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="16.100000000000001"/>
@@ -2557,95 +2560,95 @@
       <c r="A63" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B63" s="13" t="s">
         <v>61</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="21.05">
       <c r="A64" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B64" s="13" t="s">
         <v>62</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="21.05">
       <c r="A65" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="B65" s="13" t="s">
         <v>63</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="21.05">
       <c r="A66" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B66" s="6" t="s">
+      <c r="B66" s="13" t="s">
         <v>64</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="21.05">
       <c r="A67" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B67" s="6" t="s">
+      <c r="B67" s="13" t="s">
         <v>65</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="21.05">
       <c r="A68" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B68" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="B68" s="16" t="s">
         <v>66</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="21.05">
       <c r="A69" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B69" s="6" t="s">
+      <c r="B69" s="13" t="s">
         <v>67</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="21.05">
       <c r="A70" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B70" s="6" t="s">
+      <c r="B70" s="13" t="s">
         <v>68</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="21.05">
       <c r="A71" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B71" s="6" t="s">
+      <c r="B71" s="13" t="s">
         <v>69</v>
       </c>
       <c r="C71" s="11" t="s">
@@ -2689,11 +2692,11 @@
       <c r="A75" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B75" s="6" t="s">
+      <c r="B75" s="13" t="s">
         <v>73</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="21.05">

</xml_diff>

<commit_message>
Fifth Day of DSA Series
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rinku\Desktop\coding\FAANG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C2F115-686D-44C9-8DEE-DA4947B0C4A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56316754-C465-4BC6-9CB0-A5E1B02374A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1919,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="16.100000000000001"/>
@@ -2652,40 +2652,40 @@
         <v>69</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="21.05">
       <c r="A72" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B72" s="6" t="s">
+      <c r="B72" s="13" t="s">
         <v>70</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="21.05">
       <c r="A73" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B73" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="B73" s="16" t="s">
         <v>71</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="21.05">
       <c r="A74" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B74" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="B74" s="16" t="s">
         <v>72</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="21.05">
@@ -2703,44 +2703,44 @@
       <c r="A76" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B76" s="6" t="s">
+      <c r="B76" s="13" t="s">
         <v>74</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="21.05">
       <c r="A77" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B77" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="B77" s="16" t="s">
         <v>75</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="21.05">
       <c r="A78" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B78" s="6" t="s">
+      <c r="B78" s="13" t="s">
         <v>76</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="21.05">
       <c r="A79" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B79" s="6" t="s">
+      <c r="B79" s="13" t="s">
         <v>77</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="21.05">
@@ -2758,44 +2758,44 @@
       <c r="A81" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B81" s="6" t="s">
+      <c r="B81" s="13" t="s">
         <v>79</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="21.05">
       <c r="A82" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B82" s="6" t="s">
+      <c r="B82" s="13" t="s">
         <v>80</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="21.05">
       <c r="A83" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B83" s="6" t="s">
+      <c r="B83" s="13" t="s">
         <v>81</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="21.05">
       <c r="A84" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B84" s="6" t="s">
+      <c r="B84" s="13" t="s">
         <v>82</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="21.05">

</xml_diff>

<commit_message>
Sixth Day of DSA series
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rinku\Desktop\coding\FAANG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56316754-C465-4BC6-9CB0-A5E1B02374A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7317A283-19A4-49F0-BC44-5624CE9D5C69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1917,10 +1917,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
-  <dimension ref="A1:C501"/>
+  <dimension ref="A1:D501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="16.100000000000001"/>
@@ -1930,17 +1930,17 @@
     <col min="3" max="3" width="27.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="25.5">
+    <row r="1" spans="1:4" ht="25.5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="B2" s="10" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="21.05">
+    <row r="4" spans="1:4" ht="21.05">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1951,10 +1951,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" ht="21.05">
+    <row r="6" spans="1:4" ht="21.05">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -1964,8 +1964,11 @@
       <c r="C6" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="21.05">
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="21.05">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -1975,8 +1978,11 @@
       <c r="C7" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="21.05">
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="21.05">
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
@@ -1986,8 +1992,11 @@
       <c r="C8" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="21.05">
+      <c r="D8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="21.05">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -1997,8 +2006,11 @@
       <c r="C9" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="21.05">
+      <c r="D9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="21.05">
       <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
@@ -2008,8 +2020,11 @@
       <c r="C10" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="21.05">
+      <c r="D10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="21.05">
       <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
@@ -2019,8 +2034,11 @@
       <c r="C11" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="21.05">
+      <c r="D11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="21.05">
       <c r="A12" s="5" t="s">
         <v>5</v>
       </c>
@@ -2030,8 +2048,11 @@
       <c r="C12" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="21.05">
+      <c r="D12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="21.05">
       <c r="A13" s="5" t="s">
         <v>5</v>
       </c>
@@ -2041,8 +2062,11 @@
       <c r="C13" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="21.05">
+      <c r="D13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="21.05">
       <c r="A14" s="5" t="s">
         <v>466</v>
       </c>
@@ -2052,8 +2076,11 @@
       <c r="C14" s="11" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="21.05">
+      <c r="D14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="21.05">
       <c r="A15" s="5" t="s">
         <v>466</v>
       </c>
@@ -2063,8 +2090,11 @@
       <c r="C15" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="21.05">
+      <c r="D15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="21.05">
       <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
@@ -2074,8 +2104,11 @@
       <c r="C16" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="21.05">
+      <c r="D16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="21.05">
       <c r="A17" s="5" t="s">
         <v>468</v>
       </c>
@@ -2085,8 +2118,11 @@
       <c r="C17" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="21.05">
+      <c r="D17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="21.05">
       <c r="A18" s="5" t="s">
         <v>5</v>
       </c>
@@ -2096,8 +2132,11 @@
       <c r="C18" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="21.05">
+      <c r="D18">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="21.05">
       <c r="A19" s="5" t="s">
         <v>5</v>
       </c>
@@ -2107,8 +2146,11 @@
       <c r="C19" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="21.05">
+      <c r="D19">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="21.05">
       <c r="A20" s="5" t="s">
         <v>5</v>
       </c>
@@ -2118,8 +2160,11 @@
       <c r="C20" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="21.05">
+      <c r="D20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="21.05">
       <c r="A21" s="5" t="s">
         <v>5</v>
       </c>
@@ -2129,8 +2174,11 @@
       <c r="C21" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="21.05">
+      <c r="D21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="21.05">
       <c r="A22" s="5" t="s">
         <v>5</v>
       </c>
@@ -2140,8 +2188,11 @@
       <c r="C22" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="21.05">
+      <c r="D22">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="21.05">
       <c r="A23" s="5" t="s">
         <v>5</v>
       </c>
@@ -2151,8 +2202,11 @@
       <c r="C23" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="21.05">
+      <c r="D23">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="21.05">
       <c r="A24" s="5" t="s">
         <v>5</v>
       </c>
@@ -2162,8 +2216,11 @@
       <c r="C24" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="21.05">
+      <c r="D24">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="21.05">
       <c r="A25" s="5" t="s">
         <v>5</v>
       </c>
@@ -2173,8 +2230,11 @@
       <c r="C25" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="21.05">
+      <c r="D25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="21.05">
       <c r="A26" s="5" t="s">
         <v>5</v>
       </c>
@@ -2184,8 +2244,11 @@
       <c r="C26" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="21.05">
+      <c r="D26">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="21.05">
       <c r="A27" s="5" t="s">
         <v>5</v>
       </c>
@@ -2195,8 +2258,11 @@
       <c r="C27" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="21.05">
+      <c r="D27">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="21.05">
       <c r="A28" s="5" t="s">
         <v>5</v>
       </c>
@@ -2206,8 +2272,11 @@
       <c r="C28" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="21.05">
+      <c r="D28">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="21.05">
       <c r="A29" s="5" t="s">
         <v>5</v>
       </c>
@@ -2217,8 +2286,11 @@
       <c r="C29" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="21.05">
+      <c r="D29">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="21.05">
       <c r="A30" s="5" t="s">
         <v>5</v>
       </c>
@@ -2228,8 +2300,11 @@
       <c r="C30" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="21.05">
+      <c r="D30">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="21.05">
       <c r="A31" s="5" t="s">
         <v>5</v>
       </c>
@@ -2239,8 +2314,11 @@
       <c r="C31" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="21.05">
+      <c r="D31">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="21.05">
       <c r="A32" s="5" t="s">
         <v>5</v>
       </c>
@@ -2250,8 +2328,11 @@
       <c r="C32" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="21.05">
+      <c r="D32">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="21.05">
       <c r="A33" s="5" t="s">
         <v>5</v>
       </c>
@@ -2261,8 +2342,11 @@
       <c r="C33" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="21.05">
+      <c r="D33">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="21.05">
       <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
@@ -2272,8 +2356,11 @@
       <c r="C34" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="21.05">
+      <c r="D34">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="21.05">
       <c r="A35" s="5" t="s">
         <v>5</v>
       </c>
@@ -2283,8 +2370,11 @@
       <c r="C35" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="21.05">
+      <c r="D35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="21.05">
       <c r="A36" s="5" t="s">
         <v>5</v>
       </c>
@@ -2294,8 +2384,11 @@
       <c r="C36" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="21.05">
+      <c r="D36">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="21.05">
       <c r="A37" s="5" t="s">
         <v>5</v>
       </c>
@@ -2305,8 +2398,11 @@
       <c r="C37" s="11" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="21.05">
+      <c r="D37">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="21.05">
       <c r="A38" s="5" t="s">
         <v>5</v>
       </c>
@@ -2316,8 +2412,11 @@
       <c r="C38" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="21.05">
+      <c r="D38">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="21.05">
       <c r="A39" s="5" t="s">
         <v>5</v>
       </c>
@@ -2327,8 +2426,11 @@
       <c r="C39" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="21.05">
+      <c r="D39">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="21.05">
       <c r="A40" s="5" t="s">
         <v>5</v>
       </c>
@@ -2338,8 +2440,11 @@
       <c r="C40" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="21.05">
+      <c r="D40">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="21.05">
       <c r="A41" s="5" t="s">
         <v>466</v>
       </c>
@@ -2349,18 +2454,21 @@
       <c r="C41" s="11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="21.05">
+      <c r="D41">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="21.05">
       <c r="A42" s="4"/>
       <c r="B42" s="7"/>
       <c r="C42" s="11"/>
     </row>
-    <row r="43" spans="1:3" ht="21.05">
+    <row r="43" spans="1:4" ht="21.05">
       <c r="A43" s="5"/>
       <c r="B43" s="7"/>
       <c r="C43" s="11"/>
     </row>
-    <row r="44" spans="1:3" ht="21.05">
+    <row r="44" spans="1:4" ht="21.05">
       <c r="A44" s="8" t="s">
         <v>42</v>
       </c>
@@ -2371,7 +2479,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="21.05">
+    <row r="45" spans="1:4" ht="21.05">
       <c r="A45" s="8" t="s">
         <v>42</v>
       </c>
@@ -2382,7 +2490,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="21.05">
+    <row r="46" spans="1:4" ht="21.05">
       <c r="A46" s="8" t="s">
         <v>42</v>
       </c>
@@ -2393,7 +2501,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="21.05">
+    <row r="47" spans="1:4" ht="21.05">
       <c r="A47" s="8" t="s">
         <v>42</v>
       </c>
@@ -2404,7 +2512,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="21.05">
+    <row r="48" spans="1:4" ht="21.05">
       <c r="A48" s="8" t="s">
         <v>42</v>
       </c>
@@ -2747,11 +2855,11 @@
       <c r="A80" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B80" s="6" t="s">
+      <c r="B80" s="16" t="s">
         <v>78</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>4</v>
+        <v>471</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="21.05">
@@ -2802,154 +2910,154 @@
       <c r="A85" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B85" s="6" t="s">
+      <c r="B85" s="13" t="s">
         <v>83</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="21.05">
       <c r="A86" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B86" s="6" t="s">
+      <c r="B86" s="13" t="s">
         <v>84</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="21.05">
       <c r="A87" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B87" s="6" t="s">
+      <c r="B87" s="13" t="s">
         <v>85</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="21.05">
       <c r="A88" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B88" s="6" t="s">
+      <c r="B88" s="13" t="s">
         <v>86</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="21.05">
       <c r="A89" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B89" s="6" t="s">
+      <c r="B89" s="13" t="s">
         <v>87</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="21.05">
       <c r="A90" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B90" s="6" t="s">
+      <c r="B90" s="13" t="s">
         <v>88</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="21.05">
       <c r="A91" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B91" s="6" t="s">
+      <c r="B91" s="13" t="s">
         <v>89</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="21.05">
       <c r="A92" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B92" s="6" t="s">
+      <c r="B92" s="13" t="s">
         <v>90</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="21.05">
       <c r="A93" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B93" s="6" t="s">
+      <c r="B93" s="13" t="s">
         <v>91</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="21.05">
       <c r="A94" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B94" s="6" t="s">
+      <c r="B94" s="13" t="s">
         <v>92</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="21.05">
       <c r="A95" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B95" s="6" t="s">
+      <c r="B95" s="13" t="s">
         <v>93</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="21.05">
       <c r="A96" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B96" s="6" t="s">
+      <c r="B96" s="13" t="s">
         <v>94</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="21.05">
       <c r="A97" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B97" s="6" t="s">
+      <c r="B97" s="13" t="s">
         <v>95</v>
       </c>
       <c r="C97" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="21.05">
       <c r="A98" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B98" s="6" t="s">
+      <c r="B98" s="13" t="s">
         <v>96</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="99" spans="1:3">

</xml_diff>

<commit_message>
Seventh Day Of DSA series
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rinku\Desktop\coding\FAANG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7317A283-19A4-49F0-BC44-5624CE9D5C69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E272BC60-2139-4D89-9ED9-07A5D2F624DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="474">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1444,6 +1445,9 @@
   </si>
   <si>
     <t>String *</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -1919,8 +1923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B115" sqref="B115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="16.100000000000001"/>
@@ -3073,154 +3077,154 @@
       <c r="A101" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="6" t="s">
+      <c r="B101" s="13" t="s">
         <v>98</v>
       </c>
       <c r="C101" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="21.05">
       <c r="A102" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B102" s="6" t="s">
+      <c r="B102" s="13" t="s">
         <v>99</v>
       </c>
       <c r="C102" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="21.05">
       <c r="A103" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B103" s="6" t="s">
+      <c r="B103" s="13" t="s">
         <v>100</v>
       </c>
       <c r="C103" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="21.05">
       <c r="A104" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B104" s="6" t="s">
+      <c r="B104" s="13" t="s">
         <v>101</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="21.05">
       <c r="A105" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B105" s="6" t="s">
+      <c r="B105" s="13" t="s">
         <v>102</v>
       </c>
       <c r="C105" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="21.05">
       <c r="A106" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B106" s="6" t="s">
+      <c r="B106" s="16" t="s">
         <v>103</v>
       </c>
       <c r="C106" s="11" t="s">
-        <v>4</v>
+        <v>473</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="21.05">
       <c r="A107" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B107" s="6" t="s">
+      <c r="B107" s="13" t="s">
         <v>104</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="21.05">
       <c r="A108" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B108" s="6" t="s">
+      <c r="B108" s="13" t="s">
         <v>105</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="21.05">
       <c r="A109" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B109" s="6" t="s">
+      <c r="B109" s="13" t="s">
         <v>106</v>
       </c>
       <c r="C109" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="21.05">
       <c r="A110" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B110" s="6" t="s">
+      <c r="B110" s="13" t="s">
         <v>107</v>
       </c>
       <c r="C110" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="21.05">
       <c r="A111" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B111" s="6" t="s">
+      <c r="B111" s="13" t="s">
         <v>108</v>
       </c>
       <c r="C111" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="21.05">
       <c r="A112" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B112" s="6" t="s">
+      <c r="B112" s="13" t="s">
         <v>109</v>
       </c>
       <c r="C112" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="21.05">
       <c r="A113" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B113" s="6" t="s">
+      <c r="B113" s="13" t="s">
         <v>110</v>
       </c>
       <c r="C113" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="21.05">
       <c r="A114" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B114" s="6" t="s">
+      <c r="B114" s="13" t="s">
         <v>111</v>
       </c>
       <c r="C114" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="21.05">

</xml_diff>

<commit_message>
8th day of DSA Series
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rinku\Desktop\coding\FAANG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E272BC60-2139-4D89-9ED9-07A5D2F624DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A442B738-CFC3-4EB9-A080-B9ECC1FEB16A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="475">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1448,13 +1447,16 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>Searching &amp; Sorting *</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1547,6 +1549,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1569,7 +1579,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1606,6 +1616,7 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1923,8 +1934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B115" sqref="B115"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C127" sqref="C127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="16.100000000000001"/>
@@ -2648,7 +2659,7 @@
     </row>
     <row r="61" spans="1:3" ht="21.05">
       <c r="A61" s="5" t="s">
-        <v>53</v>
+        <v>472</v>
       </c>
       <c r="B61" s="16" t="s">
         <v>59</v>
@@ -2857,7 +2868,7 @@
     </row>
     <row r="80" spans="1:3" ht="21.05">
       <c r="A80" s="5" t="s">
-        <v>53</v>
+        <v>472</v>
       </c>
       <c r="B80" s="16" t="s">
         <v>78</v>
@@ -3130,7 +3141,7 @@
     </row>
     <row r="106" spans="1:3" ht="21.05">
       <c r="A106" s="5" t="s">
-        <v>97</v>
+        <v>474</v>
       </c>
       <c r="B106" s="16" t="s">
         <v>103</v>
@@ -3231,176 +3242,176 @@
       <c r="A115" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B115" s="6" t="s">
+      <c r="B115" s="13" t="s">
         <v>112</v>
       </c>
       <c r="C115" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="21.05">
       <c r="A116" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B116" s="6" t="s">
+      <c r="B116" s="18" t="s">
         <v>113</v>
       </c>
       <c r="C116" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="21.05">
       <c r="A117" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B117" s="6" t="s">
+      <c r="B117" s="13" t="s">
         <v>114</v>
       </c>
       <c r="C117" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="21.05">
       <c r="A118" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B118" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="B118" s="16" t="s">
         <v>115</v>
       </c>
       <c r="C118" s="11" t="s">
-        <v>4</v>
+        <v>473</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="21.05">
       <c r="A119" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B119" s="6" t="s">
+      <c r="B119" s="13" t="s">
         <v>116</v>
       </c>
       <c r="C119" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="21.05">
       <c r="A120" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B120" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="B120" s="16" t="s">
         <v>117</v>
       </c>
       <c r="C120" s="11" t="s">
-        <v>4</v>
+        <v>473</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="21.05">
       <c r="A121" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B121" s="6" t="s">
+      <c r="B121" s="13" t="s">
         <v>118</v>
       </c>
       <c r="C121" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="21.05">
       <c r="A122" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B122" s="6" t="s">
+      <c r="B122" s="13" t="s">
         <v>119</v>
       </c>
       <c r="C122" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="21.05">
       <c r="A123" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B123" s="6" t="s">
+      <c r="B123" s="13" t="s">
         <v>120</v>
       </c>
       <c r="C123" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="21.05">
       <c r="A124" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B124" s="6" t="s">
+      <c r="B124" s="13" t="s">
         <v>121</v>
       </c>
       <c r="C124" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="21.05">
       <c r="A125" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B125" s="6" t="s">
+      <c r="B125" s="13" t="s">
         <v>122</v>
       </c>
       <c r="C125" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="21.05">
       <c r="A126" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B126" s="6" t="s">
+      <c r="B126" s="13" t="s">
         <v>123</v>
       </c>
       <c r="C126" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="21.05">
       <c r="A127" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B127" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="B127" s="16" t="s">
         <v>124</v>
       </c>
       <c r="C127" s="11" t="s">
-        <v>4</v>
+        <v>473</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="21.05">
       <c r="A128" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B128" s="6" t="s">
+      <c r="B128" s="13" t="s">
         <v>125</v>
       </c>
       <c r="C128" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="21.05">
       <c r="A129" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B129" s="6" t="s">
+      <c r="B129" s="13" t="s">
         <v>126</v>
       </c>
       <c r="C129" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="21.05">
       <c r="A130" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B130" s="6" t="s">
+      <c r="B130" s="13" t="s">
         <v>127</v>
       </c>
       <c r="C130" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="21.05">

</xml_diff>

<commit_message>
9th Day of DSA Series
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rinku\Desktop\coding\FAANG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A442B738-CFC3-4EB9-A080-B9ECC1FEB16A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1D1AF6-7470-4884-8926-5BEE98D440C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1934,8 +1934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C127" sqref="C127"/>
+    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C149" sqref="C149:C150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="16.100000000000001"/>
@@ -1979,7 +1979,7 @@
       <c r="C6" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="4">
         <v>1</v>
       </c>
     </row>
@@ -1993,7 +1993,7 @@
       <c r="C7" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="4">
         <v>2</v>
       </c>
     </row>
@@ -2007,7 +2007,7 @@
       <c r="C8" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="4">
         <v>3</v>
       </c>
     </row>
@@ -2021,7 +2021,7 @@
       <c r="C9" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <v>4</v>
       </c>
     </row>
@@ -2035,7 +2035,7 @@
       <c r="C10" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="4">
         <v>5</v>
       </c>
     </row>
@@ -2049,7 +2049,7 @@
       <c r="C11" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="4">
         <v>6</v>
       </c>
     </row>
@@ -2063,7 +2063,7 @@
       <c r="C12" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="4">
         <v>7</v>
       </c>
     </row>
@@ -2077,7 +2077,7 @@
       <c r="C13" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="4">
         <v>8</v>
       </c>
     </row>
@@ -2091,7 +2091,7 @@
       <c r="C14" s="11" t="s">
         <v>467</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="4">
         <v>9</v>
       </c>
     </row>
@@ -2105,7 +2105,7 @@
       <c r="C15" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="4">
         <v>10</v>
       </c>
     </row>
@@ -2119,7 +2119,7 @@
       <c r="C16" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="4">
         <v>11</v>
       </c>
     </row>
@@ -2133,7 +2133,7 @@
       <c r="C17" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="4">
         <v>12</v>
       </c>
     </row>
@@ -2147,7 +2147,7 @@
       <c r="C18" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="4">
         <v>13</v>
       </c>
     </row>
@@ -2161,7 +2161,7 @@
       <c r="C19" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="4">
         <v>14</v>
       </c>
     </row>
@@ -2175,7 +2175,7 @@
       <c r="C20" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="4">
         <v>15</v>
       </c>
     </row>
@@ -2189,7 +2189,7 @@
       <c r="C21" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="4">
         <v>16</v>
       </c>
     </row>
@@ -2203,7 +2203,7 @@
       <c r="C22" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="4">
         <v>17</v>
       </c>
     </row>
@@ -2217,7 +2217,7 @@
       <c r="C23" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="4">
         <v>18</v>
       </c>
     </row>
@@ -2231,7 +2231,7 @@
       <c r="C24" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="4">
         <v>19</v>
       </c>
     </row>
@@ -2245,7 +2245,7 @@
       <c r="C25" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="4">
         <v>20</v>
       </c>
     </row>
@@ -2259,7 +2259,7 @@
       <c r="C26" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="4">
         <v>21</v>
       </c>
     </row>
@@ -2273,7 +2273,7 @@
       <c r="C27" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="4">
         <v>22</v>
       </c>
     </row>
@@ -2287,7 +2287,7 @@
       <c r="C28" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="4">
         <v>23</v>
       </c>
     </row>
@@ -2301,7 +2301,7 @@
       <c r="C29" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="4">
         <v>24</v>
       </c>
     </row>
@@ -2315,7 +2315,7 @@
       <c r="C30" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="4">
         <v>25</v>
       </c>
     </row>
@@ -2329,7 +2329,7 @@
       <c r="C31" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="4">
         <v>26</v>
       </c>
     </row>
@@ -2343,7 +2343,7 @@
       <c r="C32" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="4">
         <v>27</v>
       </c>
     </row>
@@ -2357,7 +2357,7 @@
       <c r="C33" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="4">
         <v>28</v>
       </c>
     </row>
@@ -2371,7 +2371,7 @@
       <c r="C34" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="4">
         <v>29</v>
       </c>
     </row>
@@ -2385,7 +2385,7 @@
       <c r="C35" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="4">
         <v>30</v>
       </c>
     </row>
@@ -2399,7 +2399,7 @@
       <c r="C36" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="4">
         <v>31</v>
       </c>
     </row>
@@ -2413,7 +2413,7 @@
       <c r="C37" s="11" t="s">
         <v>469</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="4">
         <v>32</v>
       </c>
     </row>
@@ -2427,7 +2427,7 @@
       <c r="C38" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="4">
         <v>33</v>
       </c>
     </row>
@@ -2441,7 +2441,7 @@
       <c r="C39" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="4">
         <v>34</v>
       </c>
     </row>
@@ -2455,7 +2455,7 @@
       <c r="C40" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="4">
         <v>35</v>
       </c>
     </row>
@@ -2469,7 +2469,7 @@
       <c r="C41" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="4">
         <v>36</v>
       </c>
     </row>
@@ -2477,11 +2477,13 @@
       <c r="A42" s="4"/>
       <c r="B42" s="7"/>
       <c r="C42" s="11"/>
+      <c r="D42" s="4"/>
     </row>
     <row r="43" spans="1:4" ht="21.05">
       <c r="A43" s="5"/>
       <c r="B43" s="7"/>
       <c r="C43" s="11"/>
+      <c r="D43" s="4"/>
     </row>
     <row r="44" spans="1:4" ht="21.05">
       <c r="A44" s="8" t="s">
@@ -3418,66 +3420,66 @@
       <c r="A131" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B131" s="6" t="s">
+      <c r="B131" s="13" t="s">
         <v>128</v>
       </c>
       <c r="C131" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="21.05">
       <c r="A132" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B132" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="B132" s="16" t="s">
         <v>129</v>
       </c>
       <c r="C132" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="21.05">
       <c r="A133" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B133" s="6" t="s">
+      <c r="B133" s="16" t="s">
         <v>130</v>
       </c>
       <c r="C133" s="11" t="s">
-        <v>4</v>
+        <v>473</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="21.05">
       <c r="A134" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B134" s="6" t="s">
+      <c r="B134" s="13" t="s">
         <v>131</v>
       </c>
       <c r="C134" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="21.05">
       <c r="A135" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B135" s="6" t="s">
+      <c r="B135" s="13" t="s">
         <v>132</v>
       </c>
       <c r="C135" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="21.05">
       <c r="A136" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B136" s="6" t="s">
+      <c r="B136" s="13" t="s">
         <v>133</v>
       </c>
       <c r="C136" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -3493,132 +3495,132 @@
       <c r="A139" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="6" t="s">
+      <c r="B139" s="13" t="s">
         <v>135</v>
       </c>
       <c r="C139" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="21.05">
       <c r="A140" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B140" s="6" t="s">
+      <c r="B140" s="13" t="s">
         <v>136</v>
       </c>
       <c r="C140" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="21.05">
       <c r="A141" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B141" s="6" t="s">
+      <c r="B141" s="13" t="s">
         <v>137</v>
       </c>
       <c r="C141" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="21.05">
       <c r="A142" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B142" s="6" t="s">
+      <c r="B142" s="13" t="s">
         <v>138</v>
       </c>
       <c r="C142" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="21.05">
       <c r="A143" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B143" s="6" t="s">
+      <c r="B143" s="13" t="s">
         <v>139</v>
       </c>
       <c r="C143" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="21.05">
       <c r="A144" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B144" s="6" t="s">
+      <c r="B144" s="13" t="s">
         <v>140</v>
       </c>
       <c r="C144" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="21.05">
       <c r="A145" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B145" s="6" t="s">
+      <c r="B145" s="13" t="s">
         <v>141</v>
       </c>
       <c r="C145" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="21.05">
       <c r="A146" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B146" s="6" t="s">
+      <c r="B146" s="13" t="s">
         <v>142</v>
       </c>
       <c r="C146" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="21.05">
       <c r="A147" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B147" s="6" t="s">
+      <c r="B147" s="13" t="s">
         <v>143</v>
       </c>
       <c r="C147" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="21.05">
       <c r="A148" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B148" s="6" t="s">
+      <c r="B148" s="13" t="s">
         <v>144</v>
       </c>
       <c r="C148" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="21.05">
       <c r="A149" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B149" s="6" t="s">
+      <c r="B149" s="13" t="s">
         <v>145</v>
       </c>
       <c r="C149" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="21.05">
       <c r="A150" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B150" s="6" t="s">
+      <c r="B150" s="13" t="s">
         <v>146</v>
       </c>
       <c r="C150" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="21.05">

</xml_diff>

<commit_message>
10th Day of DSA Series
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rinku\Desktop\coding\FAANG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1D1AF6-7470-4884-8926-5BEE98D440C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE1AC0A-B5FF-4C07-B572-C98BE62BBD95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1934,8 +1934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C149" sqref="C149:C150"/>
+    <sheetView tabSelected="1" topLeftCell="A149" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B163" sqref="B163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="16.100000000000001"/>
@@ -3627,132 +3627,132 @@
       <c r="A151" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B151" s="6" t="s">
+      <c r="B151" s="13" t="s">
         <v>147</v>
       </c>
       <c r="C151" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="21.05">
       <c r="A152" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B152" s="6" t="s">
+      <c r="B152" s="16" t="s">
         <v>148</v>
       </c>
       <c r="C152" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="21.05">
       <c r="A153" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B153" s="6" t="s">
+      <c r="B153" s="13" t="s">
         <v>149</v>
       </c>
       <c r="C153" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="21.05">
       <c r="A154" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B154" s="6" t="s">
+      <c r="B154" s="13" t="s">
         <v>150</v>
       </c>
       <c r="C154" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="21.05">
       <c r="A155" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B155" s="6" t="s">
+      <c r="B155" s="13" t="s">
         <v>151</v>
       </c>
       <c r="C155" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="21.05">
       <c r="A156" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B156" s="6" t="s">
+      <c r="B156" s="13" t="s">
         <v>152</v>
       </c>
       <c r="C156" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="21.05">
       <c r="A157" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B157" s="6" t="s">
+      <c r="B157" s="13" t="s">
         <v>153</v>
       </c>
       <c r="C157" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="21.05">
       <c r="A158" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B158" s="6" t="s">
+      <c r="B158" s="13" t="s">
         <v>154</v>
       </c>
       <c r="C158" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="21.05">
       <c r="A159" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B159" s="6" t="s">
+      <c r="B159" s="13" t="s">
         <v>155</v>
       </c>
       <c r="C159" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="21.05">
       <c r="A160" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B160" s="6" t="s">
+      <c r="B160" s="13" t="s">
         <v>156</v>
       </c>
       <c r="C160" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="21.05">
       <c r="A161" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B161" s="6" t="s">
+      <c r="B161" s="13" t="s">
         <v>157</v>
       </c>
       <c r="C161" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="21.05">
       <c r="A162" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B162" s="6" t="s">
+      <c r="B162" s="13" t="s">
         <v>158</v>
       </c>
       <c r="C162" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="21.05">
@@ -3770,7 +3770,7 @@
       <c r="A164" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B164" s="7" t="s">
+      <c r="B164" s="17" t="s">
         <v>160</v>
       </c>
       <c r="C164" s="11" t="s">
@@ -3781,11 +3781,11 @@
       <c r="A165" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B165" s="7" t="s">
+      <c r="B165" s="17" t="s">
         <v>161</v>
       </c>
       <c r="C165" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="21.05">

</xml_diff>

<commit_message>
11th day of DSA series
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rinku\Desktop\coding\FAANG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE1AC0A-B5FF-4C07-B572-C98BE62BBD95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20C5C83-4092-4981-A6D6-A78C07396BCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1558,12 +1558,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA5454"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1579,7 +1591,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1617,6 +1629,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1624,6 +1642,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFA5454"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1934,8 +1957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A149" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B163" sqref="B163"/>
+    <sheetView tabSelected="1" topLeftCell="A169" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C181" sqref="C181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="16.100000000000001"/>
@@ -1976,7 +1999,7 @@
       <c r="B6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D6" s="4">
@@ -1990,7 +2013,7 @@
       <c r="B7" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D7" s="4">
@@ -2004,7 +2027,7 @@
       <c r="B8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D8" s="4">
@@ -2018,7 +2041,7 @@
       <c r="B9" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D9" s="4">
@@ -2032,7 +2055,7 @@
       <c r="B10" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D10" s="4">
@@ -2046,7 +2069,7 @@
       <c r="B11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D11" s="4">
@@ -2060,7 +2083,7 @@
       <c r="B12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D12" s="4">
@@ -2074,7 +2097,7 @@
       <c r="B13" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D13" s="4">
@@ -2088,7 +2111,7 @@
       <c r="B14" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="20" t="s">
         <v>467</v>
       </c>
       <c r="D14" s="4">
@@ -2102,7 +2125,7 @@
       <c r="B15" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="20" t="s">
         <v>465</v>
       </c>
       <c r="D15" s="4">
@@ -2116,7 +2139,7 @@
       <c r="B16" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D16" s="4">
@@ -2130,7 +2153,7 @@
       <c r="B17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="20" t="s">
         <v>465</v>
       </c>
       <c r="D17" s="4">
@@ -2144,7 +2167,7 @@
       <c r="B18" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D18" s="4">
@@ -2158,7 +2181,7 @@
       <c r="B19" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D19" s="4">
@@ -2172,7 +2195,7 @@
       <c r="B20" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D20" s="4">
@@ -2186,7 +2209,7 @@
       <c r="B21" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D21" s="4">
@@ -2200,7 +2223,7 @@
       <c r="B22" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D22" s="4">
@@ -2214,7 +2237,7 @@
       <c r="B23" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D23" s="4">
@@ -2228,7 +2251,7 @@
       <c r="B24" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D24" s="4">
@@ -2242,7 +2265,7 @@
       <c r="B25" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D25" s="4">
@@ -2256,7 +2279,7 @@
       <c r="B26" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D26" s="4">
@@ -2270,7 +2293,7 @@
       <c r="B27" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D27" s="4">
@@ -2284,7 +2307,7 @@
       <c r="B28" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D28" s="4">
@@ -2298,7 +2321,7 @@
       <c r="B29" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D29" s="4">
@@ -2312,7 +2335,7 @@
       <c r="B30" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D30" s="4">
@@ -2326,7 +2349,7 @@
       <c r="B31" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D31" s="4">
@@ -2340,7 +2363,7 @@
       <c r="B32" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D32" s="4">
@@ -2354,7 +2377,7 @@
       <c r="B33" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D33" s="4">
@@ -2368,7 +2391,7 @@
       <c r="B34" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D34" s="4">
@@ -2382,7 +2405,7 @@
       <c r="B35" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D35" s="4">
@@ -2396,7 +2419,7 @@
       <c r="B36" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D36" s="4">
@@ -2410,7 +2433,7 @@
       <c r="B37" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="20" t="s">
         <v>469</v>
       </c>
       <c r="D37" s="4">
@@ -2424,7 +2447,7 @@
       <c r="B38" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D38" s="4">
@@ -2438,7 +2461,7 @@
       <c r="B39" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D39" s="4">
@@ -2452,7 +2475,7 @@
       <c r="B40" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="19" t="s">
         <v>465</v>
       </c>
       <c r="D40" s="4">
@@ -2466,7 +2489,7 @@
       <c r="B41" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="20" t="s">
         <v>465</v>
       </c>
       <c r="D41" s="4">
@@ -2476,13 +2499,13 @@
     <row r="42" spans="1:4" ht="21.05">
       <c r="A42" s="4"/>
       <c r="B42" s="7"/>
-      <c r="C42" s="11"/>
+      <c r="C42" s="19"/>
       <c r="D42" s="4"/>
     </row>
     <row r="43" spans="1:4" ht="21.05">
       <c r="A43" s="5"/>
       <c r="B43" s="7"/>
-      <c r="C43" s="11"/>
+      <c r="C43" s="19"/>
       <c r="D43" s="4"/>
     </row>
     <row r="44" spans="1:4" ht="21.05">
@@ -2492,7 +2515,7 @@
       <c r="B44" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2503,7 +2526,7 @@
       <c r="B45" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2514,7 +2537,7 @@
       <c r="B46" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2525,7 +2548,7 @@
       <c r="B47" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2536,7 +2559,7 @@
       <c r="B48" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2547,7 +2570,7 @@
       <c r="B49" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="C49" s="20" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2558,7 +2581,7 @@
       <c r="B50" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="C50" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2569,7 +2592,7 @@
       <c r="B51" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C51" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2580,7 +2603,7 @@
       <c r="B52" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="C52" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2591,18 +2614,18 @@
       <c r="B53" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C53" s="19" t="s">
         <v>465</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="4"/>
-      <c r="C54" s="11"/>
+      <c r="C54" s="19"/>
     </row>
     <row r="55" spans="1:3" ht="21.05">
       <c r="A55" s="5"/>
       <c r="B55" s="7"/>
-      <c r="C55" s="11"/>
+      <c r="C55" s="19"/>
     </row>
     <row r="56" spans="1:3" ht="21.05">
       <c r="A56" s="5" t="s">
@@ -2611,7 +2634,7 @@
       <c r="B56" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C56" s="11" t="s">
+      <c r="C56" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2622,7 +2645,7 @@
       <c r="B57" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C57" s="11" t="s">
+      <c r="C57" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2633,7 +2656,7 @@
       <c r="B58" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C58" s="11" t="s">
+      <c r="C58" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2644,7 +2667,7 @@
       <c r="B59" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="C59" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2655,7 +2678,7 @@
       <c r="B60" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C60" s="11" t="s">
+      <c r="C60" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2666,7 +2689,7 @@
       <c r="B61" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="C61" s="11" t="s">
+      <c r="C61" s="20" t="s">
         <v>471</v>
       </c>
     </row>
@@ -2677,7 +2700,7 @@
       <c r="B62" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C62" s="11" t="s">
+      <c r="C62" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2688,7 +2711,7 @@
       <c r="B63" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C63" s="11" t="s">
+      <c r="C63" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2699,7 +2722,7 @@
       <c r="B64" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C64" s="11" t="s">
+      <c r="C64" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2710,7 +2733,7 @@
       <c r="B65" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C65" s="11" t="s">
+      <c r="C65" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2721,7 +2744,7 @@
       <c r="B66" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C66" s="11" t="s">
+      <c r="C66" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2732,7 +2755,7 @@
       <c r="B67" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C67" s="11" t="s">
+      <c r="C67" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2743,7 +2766,7 @@
       <c r="B68" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C68" s="11" t="s">
+      <c r="C68" s="20" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2754,7 +2777,7 @@
       <c r="B69" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C69" s="11" t="s">
+      <c r="C69" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2765,7 +2788,7 @@
       <c r="B70" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="C70" s="11" t="s">
+      <c r="C70" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2776,7 +2799,7 @@
       <c r="B71" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C71" s="11" t="s">
+      <c r="C71" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2787,7 +2810,7 @@
       <c r="B72" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C72" s="11" t="s">
+      <c r="C72" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2798,7 +2821,7 @@
       <c r="B73" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="C73" s="11" t="s">
+      <c r="C73" s="20" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2809,7 +2832,7 @@
       <c r="B74" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="C74" s="11" t="s">
+      <c r="C74" s="20" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2820,7 +2843,7 @@
       <c r="B75" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C75" s="11" t="s">
+      <c r="C75" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2831,7 +2854,7 @@
       <c r="B76" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C76" s="11" t="s">
+      <c r="C76" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2842,7 +2865,7 @@
       <c r="B77" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C77" s="11" t="s">
+      <c r="C77" s="20" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2853,7 +2876,7 @@
       <c r="B78" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="C78" s="11" t="s">
+      <c r="C78" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2864,7 +2887,7 @@
       <c r="B79" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="C79" s="11" t="s">
+      <c r="C79" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2875,7 +2898,7 @@
       <c r="B80" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="C80" s="11" t="s">
+      <c r="C80" s="20" t="s">
         <v>471</v>
       </c>
     </row>
@@ -2886,7 +2909,7 @@
       <c r="B81" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C81" s="11" t="s">
+      <c r="C81" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2897,7 +2920,7 @@
       <c r="B82" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C82" s="11" t="s">
+      <c r="C82" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2908,7 +2931,7 @@
       <c r="B83" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C83" s="11" t="s">
+      <c r="C83" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2919,7 +2942,7 @@
       <c r="B84" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="C84" s="11" t="s">
+      <c r="C84" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2930,7 +2953,7 @@
       <c r="B85" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C85" s="11" t="s">
+      <c r="C85" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2941,7 +2964,7 @@
       <c r="B86" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C86" s="11" t="s">
+      <c r="C86" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2952,7 +2975,7 @@
       <c r="B87" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C87" s="11" t="s">
+      <c r="C87" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2963,7 +2986,7 @@
       <c r="B88" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="C88" s="11" t="s">
+      <c r="C88" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2974,7 +2997,7 @@
       <c r="B89" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="C89" s="11" t="s">
+      <c r="C89" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2985,7 +3008,7 @@
       <c r="B90" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="C90" s="11" t="s">
+      <c r="C90" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2996,7 +3019,7 @@
       <c r="B91" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="C91" s="11" t="s">
+      <c r="C91" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3007,7 +3030,7 @@
       <c r="B92" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="C92" s="11" t="s">
+      <c r="C92" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3018,7 +3041,7 @@
       <c r="B93" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="C93" s="11" t="s">
+      <c r="C93" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3029,7 +3052,7 @@
       <c r="B94" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="C94" s="11" t="s">
+      <c r="C94" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3040,7 +3063,7 @@
       <c r="B95" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="C95" s="11" t="s">
+      <c r="C95" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3051,7 +3074,7 @@
       <c r="B96" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="C96" s="11" t="s">
+      <c r="C96" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3062,7 +3085,7 @@
       <c r="B97" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="C97" s="11" t="s">
+      <c r="C97" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3073,7 +3096,7 @@
       <c r="B98" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="C98" s="11" t="s">
+      <c r="C98" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3093,7 +3116,7 @@
       <c r="B101" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="C101" s="11" t="s">
+      <c r="C101" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3104,7 +3127,7 @@
       <c r="B102" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="C102" s="11" t="s">
+      <c r="C102" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3115,7 +3138,7 @@
       <c r="B103" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C103" s="11" t="s">
+      <c r="C103" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3126,7 +3149,7 @@
       <c r="B104" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C104" s="11" t="s">
+      <c r="C104" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3137,7 +3160,7 @@
       <c r="B105" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="C105" s="11" t="s">
+      <c r="C105" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3148,7 +3171,7 @@
       <c r="B106" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C106" s="11" t="s">
+      <c r="C106" s="20" t="s">
         <v>473</v>
       </c>
     </row>
@@ -3159,7 +3182,7 @@
       <c r="B107" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="C107" s="11" t="s">
+      <c r="C107" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3170,7 +3193,7 @@
       <c r="B108" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="C108" s="11" t="s">
+      <c r="C108" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3181,7 +3204,7 @@
       <c r="B109" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="C109" s="11" t="s">
+      <c r="C109" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3192,7 +3215,7 @@
       <c r="B110" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="C110" s="11" t="s">
+      <c r="C110" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3203,7 +3226,7 @@
       <c r="B111" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="C111" s="11" t="s">
+      <c r="C111" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3214,7 +3237,7 @@
       <c r="B112" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="C112" s="11" t="s">
+      <c r="C112" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3225,7 +3248,7 @@
       <c r="B113" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="C113" s="11" t="s">
+      <c r="C113" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3236,7 +3259,7 @@
       <c r="B114" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C114" s="11" t="s">
+      <c r="C114" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3247,7 +3270,7 @@
       <c r="B115" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C115" s="11" t="s">
+      <c r="C115" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3258,7 +3281,7 @@
       <c r="B116" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="C116" s="11" t="s">
+      <c r="C116" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3269,7 +3292,7 @@
       <c r="B117" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="C117" s="11" t="s">
+      <c r="C117" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3280,7 +3303,7 @@
       <c r="B118" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="C118" s="11" t="s">
+      <c r="C118" s="20" t="s">
         <v>473</v>
       </c>
     </row>
@@ -3291,7 +3314,7 @@
       <c r="B119" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="C119" s="11" t="s">
+      <c r="C119" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3302,7 +3325,7 @@
       <c r="B120" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="C120" s="11" t="s">
+      <c r="C120" s="20" t="s">
         <v>473</v>
       </c>
     </row>
@@ -3313,7 +3336,7 @@
       <c r="B121" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="C121" s="11" t="s">
+      <c r="C121" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3324,7 +3347,7 @@
       <c r="B122" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="C122" s="11" t="s">
+      <c r="C122" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3335,7 +3358,7 @@
       <c r="B123" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="C123" s="11" t="s">
+      <c r="C123" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3346,7 +3369,7 @@
       <c r="B124" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="C124" s="11" t="s">
+      <c r="C124" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3357,7 +3380,7 @@
       <c r="B125" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="C125" s="11" t="s">
+      <c r="C125" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3368,7 +3391,7 @@
       <c r="B126" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="C126" s="11" t="s">
+      <c r="C126" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3379,7 +3402,7 @@
       <c r="B127" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="C127" s="11" t="s">
+      <c r="C127" s="20" t="s">
         <v>473</v>
       </c>
     </row>
@@ -3390,7 +3413,7 @@
       <c r="B128" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="C128" s="11" t="s">
+      <c r="C128" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3401,7 +3424,7 @@
       <c r="B129" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="C129" s="11" t="s">
+      <c r="C129" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3412,7 +3435,7 @@
       <c r="B130" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="C130" s="11" t="s">
+      <c r="C130" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3423,7 +3446,7 @@
       <c r="B131" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="C131" s="11" t="s">
+      <c r="C131" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3434,7 +3457,7 @@
       <c r="B132" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="C132" s="11" t="s">
+      <c r="C132" s="20" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3445,7 +3468,7 @@
       <c r="B133" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="C133" s="11" t="s">
+      <c r="C133" s="20" t="s">
         <v>473</v>
       </c>
     </row>
@@ -3456,7 +3479,7 @@
       <c r="B134" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="C134" s="11" t="s">
+      <c r="C134" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3467,7 +3490,7 @@
       <c r="B135" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="C135" s="11" t="s">
+      <c r="C135" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3478,7 +3501,7 @@
       <c r="B136" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="C136" s="11" t="s">
+      <c r="C136" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3498,7 +3521,7 @@
       <c r="B139" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="C139" s="11" t="s">
+      <c r="C139" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3509,7 +3532,7 @@
       <c r="B140" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C140" s="11" t="s">
+      <c r="C140" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3520,7 +3543,7 @@
       <c r="B141" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="C141" s="11" t="s">
+      <c r="C141" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3531,7 +3554,7 @@
       <c r="B142" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="C142" s="11" t="s">
+      <c r="C142" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3542,7 +3565,7 @@
       <c r="B143" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="C143" s="11" t="s">
+      <c r="C143" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3553,7 +3576,7 @@
       <c r="B144" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="C144" s="11" t="s">
+      <c r="C144" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3564,7 +3587,7 @@
       <c r="B145" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="C145" s="11" t="s">
+      <c r="C145" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3575,7 +3598,7 @@
       <c r="B146" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="C146" s="11" t="s">
+      <c r="C146" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3586,7 +3609,7 @@
       <c r="B147" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="C147" s="11" t="s">
+      <c r="C147" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3597,7 +3620,7 @@
       <c r="B148" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="C148" s="11" t="s">
+      <c r="C148" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3608,7 +3631,7 @@
       <c r="B149" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="C149" s="11" t="s">
+      <c r="C149" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3619,7 +3642,7 @@
       <c r="B150" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="C150" s="11" t="s">
+      <c r="C150" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3630,7 +3653,7 @@
       <c r="B151" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="C151" s="11" t="s">
+      <c r="C151" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3641,7 +3664,7 @@
       <c r="B152" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="C152" s="11" t="s">
+      <c r="C152" s="20" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3652,7 +3675,7 @@
       <c r="B153" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="C153" s="11" t="s">
+      <c r="C153" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3663,7 +3686,7 @@
       <c r="B154" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="C154" s="11" t="s">
+      <c r="C154" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3674,7 +3697,7 @@
       <c r="B155" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="C155" s="11" t="s">
+      <c r="C155" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3685,7 +3708,7 @@
       <c r="B156" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="C156" s="11" t="s">
+      <c r="C156" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3696,7 +3719,7 @@
       <c r="B157" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="C157" s="11" t="s">
+      <c r="C157" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3707,7 +3730,7 @@
       <c r="B158" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="C158" s="11" t="s">
+      <c r="C158" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3718,7 +3741,7 @@
       <c r="B159" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="C159" s="11" t="s">
+      <c r="C159" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3729,7 +3752,7 @@
       <c r="B160" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="C160" s="11" t="s">
+      <c r="C160" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3740,7 +3763,7 @@
       <c r="B161" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="C161" s="11" t="s">
+      <c r="C161" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3751,7 +3774,7 @@
       <c r="B162" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="C162" s="11" t="s">
+      <c r="C162" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3759,11 +3782,11 @@
       <c r="A163" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B163" s="6" t="s">
+      <c r="B163" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="C163" s="11" t="s">
-        <v>4</v>
+      <c r="C163" s="20" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="21.05">
@@ -3773,8 +3796,8 @@
       <c r="B164" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="C164" s="11" t="s">
-        <v>4</v>
+      <c r="C164" s="19" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="21.05">
@@ -3784,7 +3807,7 @@
       <c r="B165" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="C165" s="11" t="s">
+      <c r="C165" s="19" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3792,99 +3815,99 @@
       <c r="A166" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B166" s="6" t="s">
+      <c r="B166" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="C166" s="11" t="s">
-        <v>4</v>
+      <c r="C166" s="19" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="167" spans="1:3" ht="21.05">
       <c r="A167" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B167" s="6" t="s">
+      <c r="B167" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="C167" s="11" t="s">
-        <v>4</v>
+      <c r="C167" s="19" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="21.05">
       <c r="A168" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B168" s="6" t="s">
+      <c r="B168" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="C168" s="11" t="s">
-        <v>4</v>
+      <c r="C168" s="20" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="21.05">
       <c r="A169" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B169" s="6" t="s">
+      <c r="B169" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="C169" s="11" t="s">
-        <v>4</v>
+      <c r="C169" s="19" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="21.05">
       <c r="A170" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B170" s="6" t="s">
+      <c r="B170" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="C170" s="11" t="s">
-        <v>4</v>
+      <c r="C170" s="20" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="171" spans="1:3" ht="21.05">
       <c r="A171" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B171" s="6" t="s">
+      <c r="B171" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="C171" s="11" t="s">
-        <v>4</v>
+      <c r="C171" s="19" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="21.05">
       <c r="A172" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B172" s="6" t="s">
+      <c r="B172" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="C172" s="11" t="s">
-        <v>4</v>
+      <c r="C172" s="19" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="21.05">
       <c r="A173" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B173" s="6" t="s">
+      <c r="B173" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="C173" s="11" t="s">
-        <v>4</v>
+      <c r="C173" s="19" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="21.05">
       <c r="A174" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B174" s="6" t="s">
+      <c r="B174" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="C174" s="11" t="s">
-        <v>4</v>
+      <c r="C174" s="20" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -3900,55 +3923,55 @@
       <c r="A177" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="6" t="s">
+      <c r="B177" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="C177" s="11" t="s">
-        <v>4</v>
+      <c r="C177" s="19" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="21.05">
       <c r="A178" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B178" s="6" t="s">
+      <c r="B178" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="C178" s="11" t="s">
-        <v>4</v>
+      <c r="C178" s="19" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="21.05">
       <c r="A179" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B179" s="6" t="s">
+      <c r="B179" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="C179" s="11" t="s">
-        <v>4</v>
+      <c r="C179" s="19" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="21.05">
       <c r="A180" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B180" s="6" t="s">
+      <c r="B180" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="C180" s="11" t="s">
-        <v>4</v>
+      <c r="C180" s="19" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="21.05">
       <c r="A181" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B181" s="6" t="s">
+      <c r="B181" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="C181" s="11" t="s">
-        <v>4</v>
+      <c r="C181" s="19" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="21.05">

</xml_diff>

<commit_message>
12th Day of DSA Series
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rinku\Desktop\coding\FAANG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20C5C83-4092-4981-A6D6-A78C07396BCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D22647-C8DF-45CD-84A7-DE032EBD92F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1957,8 +1957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C181" sqref="C181"/>
+    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C191" sqref="C191:C192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="16.100000000000001"/>
@@ -3978,121 +3978,121 @@
       <c r="A182" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B182" s="6" t="s">
+      <c r="B182" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="C182" s="11" t="s">
-        <v>4</v>
+      <c r="C182" s="19" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="21.05">
       <c r="A183" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B183" s="6" t="s">
+      <c r="B183" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="C183" s="11" t="s">
-        <v>4</v>
+      <c r="C183" s="19" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="21.05">
       <c r="A184" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B184" s="6" t="s">
+      <c r="B184" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="C184" s="11" t="s">
-        <v>4</v>
+      <c r="C184" s="19" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="21.05">
       <c r="A185" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B185" s="6" t="s">
+      <c r="B185" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="C185" s="11" t="s">
-        <v>4</v>
+      <c r="C185" s="19" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="21.05">
       <c r="A186" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B186" s="6" t="s">
+      <c r="B186" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="C186" s="11" t="s">
-        <v>4</v>
+      <c r="C186" s="19" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="21.05">
       <c r="A187" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B187" s="6" t="s">
+      <c r="B187" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="C187" s="11" t="s">
-        <v>4</v>
+      <c r="C187" s="19" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="188" spans="1:3" ht="21.05">
       <c r="A188" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B188" s="6" t="s">
+      <c r="B188" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="C188" s="11" t="s">
-        <v>4</v>
+      <c r="C188" s="19" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="21.05">
       <c r="A189" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B189" s="6" t="s">
+      <c r="B189" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="C189" s="11" t="s">
-        <v>4</v>
+      <c r="C189" s="20" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="21.05">
       <c r="A190" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B190" s="6" t="s">
+      <c r="B190" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="C190" s="11" t="s">
-        <v>4</v>
+      <c r="C190" s="19" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="21.05">
       <c r="A191" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B191" s="6" t="s">
+      <c r="B191" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="C191" s="11" t="s">
-        <v>4</v>
+      <c r="C191" s="19" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="192" spans="1:3" ht="21.05">
       <c r="A192" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B192" s="6" t="s">
+      <c r="B192" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="C192" s="11" t="s">
-        <v>4</v>
+      <c r="C192" s="19" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="21.05">

</xml_diff>